<commit_message>
retrofitted to use ExcelFixture from the excel module
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="QuickObject" sheetId="1" r:id="rId1"/>
+    <sheet name="QuickObjectRowHandler" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +38,21 @@
   </si>
   <si>
     <t>Local Date</t>
+  </si>
+  <si>
+    <t>anInteger</t>
+  </si>
+  <si>
+    <t>aBoolean</t>
+  </si>
+  <si>
+    <t>FooViaRowHandler</t>
+  </si>
+  <si>
+    <t>BarViaRowHandler</t>
+  </si>
+  <si>
+    <t>BazViaRowHandler</t>
   </si>
 </sst>
 </file>
@@ -382,9 +398,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2">
+        <v>42016</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>222</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42094</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>333</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,18 +487,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>111</v>
@@ -422,7 +512,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>222</v>
@@ -436,7 +526,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>333</v>
@@ -448,18 +538,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -473,4 +551,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bringing in additional modules, adding a demo script
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110"/>
   </bookViews>
   <sheets>
     <sheet name="QuickObject" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Foo</t>
   </si>
@@ -31,21 +28,6 @@
     <t>Baz</t>
   </si>
   <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Local Date</t>
-  </si>
-  <si>
-    <t>anInteger</t>
-  </si>
-  <si>
-    <t>aBoolean</t>
-  </si>
-  <si>
     <t>FooViaRowHandler</t>
   </si>
   <si>
@@ -53,6 +35,18 @@
   </si>
   <si>
     <t>BazViaRowHandler</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>localDate</t>
+  </si>
+  <si>
+    <t>flag</t>
   </si>
 </sst>
 </file>
@@ -398,9 +392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,21 +405,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>111</v>
@@ -439,7 +433,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>222</v>
@@ -453,7 +447,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>333</v>
@@ -472,33 +466,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>111</v>
@@ -512,7 +507,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>222</v>
@@ -526,7 +521,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>333</v>

</xml_diff>

<commit_message>
updating DEMO-SCRIPT.adoc, also temporarily committing changes made while preparing
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/spreadsheets/QuickObjects-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QuickObject" sheetId="1" r:id="rId1"/>
@@ -392,9 +392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,9 +466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>